<commit_message>
[#5] Begin sheets reinitialization on deconstruction
</commit_message>
<xml_diff>
--- a/construct-logic/src/test/resources/org/keyboardplaying/xtt/xlsx/xlsx_test.xlsx
+++ b/construct-logic/src/test/resources/org/keyboardplaying/xtt/xlsx/xlsx_test.xlsx
@@ -7,9 +7,8 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Cfg" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -54,8 +53,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,20 +359,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -379,19 +388,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>